<commit_message>
Dữ liệu cơ quan
</commit_message>
<xml_diff>
--- a/SOMUCKE/SMKKHESANH.xlsx
+++ b/SOMUCKE/SMKKHESANH.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\8.CoQuan\SODO\SOMUCKE\SOMUCKE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CNHH\BOPHANKYTHUAT\SODO\SOMUCKE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" tabRatio="895" firstSheet="6" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12780" tabRatio="895" firstSheet="6" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="44" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <sheet name="114" sheetId="72" r:id="rId72"/>
     <sheet name="115" sheetId="73" r:id="rId73"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3529" uniqueCount="1715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="1728">
   <si>
     <t>SỐ THỬA MỚI</t>
   </si>
@@ -5276,11 +5276,50 @@
   <si>
     <t>Đặng Thị Lãnh</t>
   </si>
+  <si>
+    <t>CL thửa 366</t>
+  </si>
+  <si>
+    <t>Lê Châu Thuẩn</t>
+  </si>
+  <si>
+    <t>HT 22,23</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn Tiến</t>
+  </si>
+  <si>
+    <t>Trần Thị Thao</t>
+  </si>
+  <si>
+    <t>TT 302</t>
+  </si>
+  <si>
+    <t>CL thửa 18</t>
+  </si>
+  <si>
+    <t>đinh Phương Hồng Hạnh</t>
+  </si>
+  <si>
+    <t>HT392 và 393</t>
+  </si>
+  <si>
+    <t>Hồ Thị Phương Thảo</t>
+  </si>
+  <si>
+    <t>Hồ Đăng Ngọc</t>
+  </si>
+  <si>
+    <t>Lê Thị Hường</t>
+  </si>
+  <si>
+    <t>TT208</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -16333,10 +16372,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21"/>
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18134,6 +18173,30 @@
       </c>
       <c r="H109" s="30" t="s">
         <v>1597</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="30">
+        <v>158</v>
+      </c>
+      <c r="B110" s="30" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="30">
+        <v>159</v>
+      </c>
+      <c r="B111" s="30" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="30">
+        <v>160</v>
+      </c>
+      <c r="B112" s="30" t="s">
+        <v>749</v>
       </c>
     </row>
   </sheetData>
@@ -21250,7 +21313,7 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="A40" sqref="A40:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -21974,7 +22037,9 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
+      <c r="A41" s="4">
+        <v>364</v>
+      </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -21984,24 +22049,42 @@
       <c r="H41" s="23"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="A42" s="4">
+        <v>365</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C42" s="4">
+        <v>104.9</v>
+      </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="23"/>
+      <c r="H42" s="23" t="s">
+        <v>1358</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="A43" s="4">
+        <v>366</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C43" s="4">
+        <v>672.8</v>
+      </c>
+      <c r="D43" s="4">
+        <v>110</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="23"/>
+      <c r="H43" s="23" t="s">
+        <v>1358</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
@@ -22218,7 +22301,7 @@
   <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -23661,10 +23744,10 @@
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet27"/>
-  <dimension ref="A1:O89"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -25338,6 +25421,40 @@
       </c>
       <c r="H89" s="5" t="s">
         <v>1684</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="5">
+        <v>414</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C90" s="5">
+        <v>673.6</v>
+      </c>
+      <c r="D90" s="5">
+        <v>150</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="5">
+        <v>415</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C91" s="5">
+        <v>779.9</v>
+      </c>
+      <c r="D91" s="5">
+        <v>150</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>1727</v>
       </c>
     </row>
   </sheetData>
@@ -32858,10 +32975,10 @@
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet32"/>
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104:E106"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="H106" sqref="H106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -34725,7 +34842,7 @@
         <v>100</v>
       </c>
       <c r="E105" s="5">
-        <f t="shared" ref="E105:E106" si="0">C105-D105</f>
+        <f t="shared" ref="E105:E107" si="0">C105-D105</f>
         <v>45.5</v>
       </c>
       <c r="H105" s="5" t="s">
@@ -34751,6 +34868,27 @@
       </c>
       <c r="H106" s="5" t="s">
         <v>1709</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" s="5">
+        <v>485</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C107" s="5">
+        <v>324.8</v>
+      </c>
+      <c r="D107" s="5">
+        <v>80</v>
+      </c>
+      <c r="E107" s="5">
+        <f t="shared" si="0"/>
+        <v>244.8</v>
+      </c>
+      <c r="H107" s="5" t="s">
+        <v>1723</v>
       </c>
     </row>
   </sheetData>
@@ -34768,10 +34906,10 @@
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet33"/>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -35431,7 +35569,10 @@
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4">
+        <f t="shared" ref="E32:E36" si="0">C32-D32</f>
+        <v>0</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -35450,7 +35591,10 @@
       <c r="D33" s="4">
         <v>50</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4">
+        <f t="shared" si="0"/>
+        <v>333</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -35469,7 +35613,10 @@
       <c r="D34" s="4">
         <v>50</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4">
+        <f t="shared" si="0"/>
+        <v>341</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -35484,7 +35631,10 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -35493,37 +35643,76 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="A36" s="4">
+        <v>302</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C36" s="4">
+        <v>762.8</v>
+      </c>
+      <c r="D36" s="4">
+        <v>100</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="0"/>
+        <v>662.8</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>1721</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="A37" s="4">
+        <v>303</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C37" s="4">
+        <v>494.9</v>
+      </c>
+      <c r="D37" s="4">
+        <v>50</v>
+      </c>
+      <c r="E37" s="4">
+        <f>C37-D37</f>
+        <v>444.9</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
+      <c r="I37" s="4" t="s">
+        <v>1720</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="A38" s="4">
+        <v>304</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C38" s="4">
+        <v>267.89999999999998</v>
+      </c>
+      <c r="D38" s="4">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4">
+        <f>C38-D38</f>
+        <v>217.89999999999998</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>1720</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
@@ -35799,6 +35988,17 @@
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -35817,8 +36017,8 @@
   <sheetPr codeName="Sheet34"/>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37837,8 +38037,8 @@
   <sheetPr codeName="Sheet36"/>
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121:E123"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -44786,8 +44986,8 @@
   <sheetPr codeName="Sheet41"/>
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -47495,10 +47695,10 @@
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet42"/>
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -49090,6 +49290,34 @@
       </c>
       <c r="H92" s="5" t="s">
         <v>1671</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="5">
+        <v>369</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C93" s="5">
+        <v>313.3</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="5">
+        <v>370</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="C94" s="5">
+        <v>308.5</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>1715</v>
       </c>
     </row>
   </sheetData>
@@ -56142,7 +56370,7 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H25" activeCellId="2" sqref="H23 H24 H25"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -59604,8 +59832,8 @@
   <sheetPr codeName="Sheet50"/>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -59994,14 +60222,22 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="4">
+        <v>150</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C21" s="4">
+        <v>826.5</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>1717</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
@@ -77551,8 +77787,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78608,24 +78844,44 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="A56" s="2">
+        <v>116</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1372.1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>100</v>
+      </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>1418</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="A57" s="2">
+        <v>117</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2648.2</v>
+      </c>
+      <c r="D57" s="2">
+        <v>60</v>
+      </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
+      <c r="H57" s="2" t="s">
+        <v>1418</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>

</xml_diff>

<commit_message>
lay số tờ 70 khe sanh
</commit_message>
<xml_diff>
--- a/SOMUCKE/SMKKHESANH.xlsx
+++ b/SOMUCKE/SMKKHESANH.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12780" tabRatio="895" firstSheet="6" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12780" tabRatio="895" firstSheet="6" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="44" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3569" uniqueCount="1733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3573" uniqueCount="1736">
   <si>
     <t>SỐ THỬA MỚI</t>
   </si>
@@ -5329,6 +5329,15 @@
   </si>
   <si>
     <t>Trần Hữu Ngọc</t>
+  </si>
+  <si>
+    <t>Hoàng Văn Nam</t>
+  </si>
+  <si>
+    <t>Hoàng Văn Khánh</t>
+  </si>
+  <si>
+    <t>TT284</t>
   </si>
 </sst>
 </file>
@@ -23759,10 +23768,10 @@
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet27"/>
-  <dimension ref="A1:O91"/>
+  <dimension ref="A1:O93"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -25470,6 +25479,48 @@
       </c>
       <c r="H91" s="5" t="s">
         <v>1727</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="5">
+        <v>416</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C92" s="5">
+        <v>198.2</v>
+      </c>
+      <c r="D92" s="5">
+        <v>100</v>
+      </c>
+      <c r="G92" s="5">
+        <f>C92-D92</f>
+        <v>98.199999999999989</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="5">
+        <v>417</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C93" s="5">
+        <v>402.6</v>
+      </c>
+      <c r="D93" s="5">
+        <v>100</v>
+      </c>
+      <c r="G93" s="5">
+        <f>C93-D93</f>
+        <v>302.60000000000002</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>1735</v>
       </c>
     </row>
   </sheetData>
@@ -36129,7 +36180,7 @@
   <sheetPr codeName="Sheet34"/>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>

</xml_diff>